<commit_message>
Set up webscraping yelp
</commit_message>
<xml_diff>
--- a/web_scrape/Scraping_Sheet_Short.xlsx
+++ b/web_scrape/Scraping_Sheet_Short.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalip\OneDrive\Documents\physician_web_scraper\web_scrape\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B576BA1D-ACE9-4D49-8273-3E4750C8CEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F10316-F5D1-47EA-8237-7A0AAC469BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - American Head and Nec" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="1293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2898" uniqueCount="1293">
   <si>
     <t>ID</t>
   </si>
@@ -4516,7 +4517,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -4579,6 +4580,12 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0A0101"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -4875,7 +4882,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4994,6 +5001,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6159,8 +6172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O290"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A252" workbookViewId="0">
-      <selection activeCell="J258" sqref="J258"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="19.95" customHeight="1"/>
@@ -6622,8 +6635,8 @@
       <c r="E17" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="13" t="s">
-        <v>60</v>
+      <c r="F17" s="40" t="s">
+        <v>15</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>62</v>
@@ -7459,7 +7472,7 @@
       <c r="E48" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="F48" s="13" t="s">
+      <c r="F48" s="36" t="s">
         <v>177</v>
       </c>
       <c r="G48" s="13" t="s">
@@ -14031,7 +14044,7 @@
     <hyperlink ref="E16" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
     <hyperlink ref="D17" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
     <hyperlink ref="E17" r:id="rId26" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
-    <hyperlink ref="F17" r:id="rId27" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="F17" r:id="rId27" display="https://www.healthgrades.com/physician/dr-amy-chen-x4768" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
     <hyperlink ref="G17" r:id="rId28" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
     <hyperlink ref="D20" r:id="rId29" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
     <hyperlink ref="E20" r:id="rId30" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
@@ -14094,6 +14107,7 @@
     <hyperlink ref="E260" r:id="rId87" xr:uid="{A25DE5CC-5BFE-42A8-99E0-53E179B31C5A}"/>
     <hyperlink ref="E258" r:id="rId88" xr:uid="{6ACB97E9-307B-45F8-B41F-79B78A244BA9}"/>
     <hyperlink ref="E259" r:id="rId89" xr:uid="{94A7B252-CBC4-406E-8F21-1385A092DB5A}"/>
+    <hyperlink ref="F48" r:id="rId90" xr:uid="{5C691963-902F-4604-9F12-4A113559D4F2}"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup scale="72" orientation="portrait"/>
@@ -14101,4 +14115,3264 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27852A61-7B38-4839-9814-C6FBEBE0A2AE}">
+  <dimension ref="A1:J289"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.6">
+      <c r="A1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="41">
+        <f>COUNTIF($A$1:$B$289,"N/A")</f>
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.6">
+      <c r="A2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="13.8">
+      <c r="A3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.6">
+      <c r="A4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="13.8">
+      <c r="A5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="13.8">
+      <c r="A6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="13.8">
+      <c r="A7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.6">
+      <c r="A8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.6">
+      <c r="A9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.6">
+      <c r="A10" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="13.8">
+      <c r="A11" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="13.8">
+      <c r="A12" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="13.8">
+      <c r="A13" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="13.8">
+      <c r="A14" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="13.8">
+      <c r="A15" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.6">
+      <c r="A16" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="13.8">
+      <c r="A17" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="13.8">
+      <c r="A18" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="13.8">
+      <c r="A19" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.6">
+      <c r="A20" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="13.8">
+      <c r="A21" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.6">
+      <c r="A22" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="13.8">
+      <c r="A23" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.6">
+      <c r="A24" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.6">
+      <c r="A25" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="13.8">
+      <c r="A26" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="13.8">
+      <c r="A27" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="13.8">
+      <c r="A28" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="13.8">
+      <c r="A29" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="13.8">
+      <c r="A30" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="13.8">
+      <c r="A31" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="13.8">
+      <c r="A32" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="13.8">
+      <c r="A33" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="13.8">
+      <c r="A34" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="13.8">
+      <c r="A35" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="13.8">
+      <c r="A36" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="13.8">
+      <c r="A37" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="13.8">
+      <c r="A38" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.6">
+      <c r="A39" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="13.8">
+      <c r="A40" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.6">
+      <c r="A41" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="13.8">
+      <c r="A42" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="13.8">
+      <c r="A43" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="13.8">
+      <c r="A44" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="13.8">
+      <c r="A45" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="13.8">
+      <c r="A46" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="13.8">
+      <c r="A47" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="B47" s="36" t="s">
+        <v>177</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="13.8">
+      <c r="A48" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="13.8">
+      <c r="A49" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="13.8">
+      <c r="A50" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="13.8">
+      <c r="A51" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="13.8">
+      <c r="A52" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="13.8">
+      <c r="A53" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="13.8">
+      <c r="A54" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="13.8">
+      <c r="A55" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="13.8">
+      <c r="A56" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="13.8">
+      <c r="A57" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="13.8">
+      <c r="A58" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="13.8">
+      <c r="A59" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="13.8">
+      <c r="A60" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="13.8">
+      <c r="A61" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="13.8">
+      <c r="A62" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="13.8">
+      <c r="A63" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="13.8">
+      <c r="A64" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="13.8">
+      <c r="A65" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="13.8">
+      <c r="A66" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B66" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="13.8">
+      <c r="A67" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="B67" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="13.8">
+      <c r="A68" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B68" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C68" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="13.8">
+      <c r="A69" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="B69" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="13.8">
+      <c r="A70" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B70" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="13.8">
+      <c r="A71" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="13.8">
+      <c r="A72" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="C72" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="13.8">
+      <c r="A73" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="B73" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="13.8">
+      <c r="A74" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="13.8">
+      <c r="A75" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C75" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="13.8">
+      <c r="A76" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="13.8">
+      <c r="A77" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C77" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="13.8">
+      <c r="A78" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="C78" s="13" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="13.8">
+      <c r="A79" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="B79" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="C79" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="13.8">
+      <c r="A80" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B80" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="13.8">
+      <c r="A81" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="B81" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="13.8">
+      <c r="A82" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="13.8">
+      <c r="A83" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="B83" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="C83" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="13.8">
+      <c r="A84" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="B84" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C84" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="13.8">
+      <c r="A85" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="B85" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="13.8">
+      <c r="A86" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="B86" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="C86" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="13.8">
+      <c r="A87" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="B87" s="13" t="s">
+        <v>328</v>
+      </c>
+      <c r="C87" s="36" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="13.8">
+      <c r="A88" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B88" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="13.8">
+      <c r="A89" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="B89" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="13.8">
+      <c r="A90" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B90" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C90" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="13.8">
+      <c r="A91" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="B91" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="13.8">
+      <c r="A92" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="B92" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="C92" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="13.8">
+      <c r="A93" s="13" t="s">
+        <v>352</v>
+      </c>
+      <c r="B93" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="C93" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="13.8">
+      <c r="A94" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="B94" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="C94" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="13.8">
+      <c r="A95" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="B95" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="C95" s="13" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="13.8">
+      <c r="A96" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="B96" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="C96" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="13.8">
+      <c r="A97" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B97" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C97" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="13.8">
+      <c r="A98" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B98" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C98" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="79.2">
+      <c r="A99" s="22" t="s">
+        <v>376</v>
+      </c>
+      <c r="B99" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="79.2">
+      <c r="A100" s="23" t="s">
+        <v>379</v>
+      </c>
+      <c r="B100" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="13.8">
+      <c r="A101" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B101" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="13.8">
+      <c r="A102" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="B102" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="C102" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="13.8">
+      <c r="A103" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="B103" s="13" t="s">
+        <v>391</v>
+      </c>
+      <c r="C103" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="13.8">
+      <c r="A104" s="13" t="s">
+        <v>395</v>
+      </c>
+      <c r="B104" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="C104" s="13" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="13.8">
+      <c r="A105" s="13" t="s">
+        <v>401</v>
+      </c>
+      <c r="B105" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C105" s="13" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="13.8">
+      <c r="A106" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B106" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C106" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="13.8">
+      <c r="A107" s="13" t="s">
+        <v>407</v>
+      </c>
+      <c r="B107" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C107" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="13.8">
+      <c r="A108" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B108" s="13" t="s">
+        <v>412</v>
+      </c>
+      <c r="C108" s="13" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="13.8">
+      <c r="A109" s="13" t="s">
+        <v>416</v>
+      </c>
+      <c r="B109" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="C109" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="13.8">
+      <c r="A110" s="13" t="s">
+        <v>420</v>
+      </c>
+      <c r="B110" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C110" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="13.8">
+      <c r="A111" s="13" t="s">
+        <v>424</v>
+      </c>
+      <c r="B111" s="13" t="s">
+        <v>425</v>
+      </c>
+      <c r="C111" s="13" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="13.8">
+      <c r="A112" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="B112" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C112" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="13.8">
+      <c r="A113" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="B113" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C113" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="13.8">
+      <c r="A114" s="13" t="s">
+        <v>437</v>
+      </c>
+      <c r="B114" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C114" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="13.8">
+      <c r="A115" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B115" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C115" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="13.8">
+      <c r="A116" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B116" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C116" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="13.8">
+      <c r="A117" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="B117" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C117" s="13" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="13.8">
+      <c r="A118" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="B118" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C118" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="13.8">
+      <c r="A119" s="13" t="s">
+        <v>453</v>
+      </c>
+      <c r="B119" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C119" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="13.8">
+      <c r="A120" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B120" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C120" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="13.8">
+      <c r="A121" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B121" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C121" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="13.8">
+      <c r="A122" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="B122" s="13" t="s">
+        <v>463</v>
+      </c>
+      <c r="C122" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="13.8">
+      <c r="A123" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="B123" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="C123" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="13.8">
+      <c r="A124" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="B124" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="C124" s="13" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="13.8">
+      <c r="A125" s="13" t="s">
+        <v>475</v>
+      </c>
+      <c r="B125" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C125" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="13.8">
+      <c r="A126" s="13" t="s">
+        <v>479</v>
+      </c>
+      <c r="B126" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C126" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="13.8">
+      <c r="A127" s="13" t="s">
+        <v>483</v>
+      </c>
+      <c r="B127" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C127" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="13.8">
+      <c r="A128" s="13" t="s">
+        <v>487</v>
+      </c>
+      <c r="B128" s="13" t="s">
+        <v>488</v>
+      </c>
+      <c r="C128" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="13.8">
+      <c r="A129" s="13" t="s">
+        <v>492</v>
+      </c>
+      <c r="B129" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C129" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="13.8">
+      <c r="A130" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B130" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C130" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="13.8">
+      <c r="A131" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="B131" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C131" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="13.8">
+      <c r="A132" s="13" t="s">
+        <v>500</v>
+      </c>
+      <c r="B132" s="13" t="s">
+        <v>501</v>
+      </c>
+      <c r="C132" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="13.8">
+      <c r="A133" s="13" t="s">
+        <v>505</v>
+      </c>
+      <c r="B133" s="13" t="s">
+        <v>506</v>
+      </c>
+      <c r="C133" s="13" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="13.8">
+      <c r="A134" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B134" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C134" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="13.8">
+      <c r="A135" s="13" t="s">
+        <v>512</v>
+      </c>
+      <c r="B135" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C135" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="13.8">
+      <c r="A136" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B136" s="13" t="s">
+        <v>514</v>
+      </c>
+      <c r="C136" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="13.8">
+      <c r="A137" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="B137" s="13" t="s">
+        <v>518</v>
+      </c>
+      <c r="C137" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="13.8">
+      <c r="A138" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B138" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C138" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="13.8">
+      <c r="A139" s="13" t="s">
+        <v>522</v>
+      </c>
+      <c r="B139" s="13" t="s">
+        <v>523</v>
+      </c>
+      <c r="C139" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="13.8">
+      <c r="A140" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B140" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C140" s="13" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="13.8">
+      <c r="A141" s="13" t="s">
+        <v>530</v>
+      </c>
+      <c r="B141" s="13" t="s">
+        <v>531</v>
+      </c>
+      <c r="C141" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="13.8">
+      <c r="A142" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B142" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C142" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="13.8">
+      <c r="A143" s="13" t="s">
+        <v>537</v>
+      </c>
+      <c r="B143" s="13" t="s">
+        <v>538</v>
+      </c>
+      <c r="C143" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="13.8">
+      <c r="A144" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B144" s="13" t="s">
+        <v>542</v>
+      </c>
+      <c r="C144" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="13.8">
+      <c r="A145" s="13" t="s">
+        <v>546</v>
+      </c>
+      <c r="B145" s="13" t="s">
+        <v>547</v>
+      </c>
+      <c r="C145" s="13" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="13.8">
+      <c r="A146" s="13" t="s">
+        <v>552</v>
+      </c>
+      <c r="B146" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C146" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="13.8">
+      <c r="A147" s="13" t="s">
+        <v>536</v>
+      </c>
+      <c r="B147" s="13" t="s">
+        <v>556</v>
+      </c>
+      <c r="C147" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="13.8">
+      <c r="A148" s="13" t="s">
+        <v>560</v>
+      </c>
+      <c r="B148" s="13" t="s">
+        <v>561</v>
+      </c>
+      <c r="C148" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="13.8">
+      <c r="A149" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B149" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C149" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="13.8">
+      <c r="A150" s="13" t="s">
+        <v>566</v>
+      </c>
+      <c r="B150" s="13" t="s">
+        <v>567</v>
+      </c>
+      <c r="C150" s="13" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="13.8">
+      <c r="A151" s="13" t="s">
+        <v>572</v>
+      </c>
+      <c r="B151" s="13" t="s">
+        <v>573</v>
+      </c>
+      <c r="C151" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="13.8">
+      <c r="A152" s="13" t="s">
+        <v>577</v>
+      </c>
+      <c r="B152" s="13" t="s">
+        <v>578</v>
+      </c>
+      <c r="C152" s="13" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="13.8">
+      <c r="A153" s="13" t="s">
+        <v>583</v>
+      </c>
+      <c r="B153" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C153" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="13.8">
+      <c r="A154" s="13" t="s">
+        <v>586</v>
+      </c>
+      <c r="B154" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C154" s="13" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="13.8">
+      <c r="A155" s="13" t="s">
+        <v>591</v>
+      </c>
+      <c r="B155" s="13" t="s">
+        <v>592</v>
+      </c>
+      <c r="C155" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="13.8">
+      <c r="A156" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B156" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C156" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="13.8">
+      <c r="A157" s="25" t="s">
+        <v>597</v>
+      </c>
+      <c r="B157" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C157" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="13.8">
+      <c r="A158" s="13" t="s">
+        <v>601</v>
+      </c>
+      <c r="B158" s="25" t="s">
+        <v>602</v>
+      </c>
+      <c r="C158" s="13" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="13.8">
+      <c r="A159" s="13" t="s">
+        <v>606</v>
+      </c>
+      <c r="B159" s="25" t="s">
+        <v>607</v>
+      </c>
+      <c r="C159" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="13.8">
+      <c r="A160" s="13" t="s">
+        <v>611</v>
+      </c>
+      <c r="B160" s="25" t="s">
+        <v>612</v>
+      </c>
+      <c r="C160" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="13.8">
+      <c r="A161" s="13" t="s">
+        <v>616</v>
+      </c>
+      <c r="B161" s="13" t="s">
+        <v>617</v>
+      </c>
+      <c r="C161" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="13.8">
+      <c r="A162" s="13" t="s">
+        <v>621</v>
+      </c>
+      <c r="B162" s="25" t="s">
+        <v>622</v>
+      </c>
+      <c r="C162" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="13.8">
+      <c r="A163" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B163" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C163" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="13.8">
+      <c r="A164" s="13" t="s">
+        <v>629</v>
+      </c>
+      <c r="B164" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C164" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="13.8">
+      <c r="A165" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B165" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C165" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="13.8">
+      <c r="A166" s="13" t="s">
+        <v>635</v>
+      </c>
+      <c r="B166" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C166" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="13.8">
+      <c r="A167" s="13" t="s">
+        <v>639</v>
+      </c>
+      <c r="B167" s="13" t="s">
+        <v>640</v>
+      </c>
+      <c r="C167" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="13.8">
+      <c r="A168" s="13" t="s">
+        <v>644</v>
+      </c>
+      <c r="B168" s="13" t="s">
+        <v>645</v>
+      </c>
+      <c r="C168" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="13.8">
+      <c r="A169" s="13" t="s">
+        <v>648</v>
+      </c>
+      <c r="B169" s="25" t="s">
+        <v>649</v>
+      </c>
+      <c r="C169" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" ht="13.8">
+      <c r="A170" s="25" t="s">
+        <v>651</v>
+      </c>
+      <c r="B170" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C170" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="13.8">
+      <c r="A171" s="13" t="s">
+        <v>654</v>
+      </c>
+      <c r="B171" s="25" t="s">
+        <v>655</v>
+      </c>
+      <c r="C171" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="13.8">
+      <c r="A172" s="13" t="s">
+        <v>658</v>
+      </c>
+      <c r="B172" s="25" t="s">
+        <v>659</v>
+      </c>
+      <c r="C172" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="13.8">
+      <c r="A173" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B173" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C173" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" ht="13.8">
+      <c r="A174" s="13" t="s">
+        <v>665</v>
+      </c>
+      <c r="B174" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C174" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="13.8">
+      <c r="A175" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B175" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C175" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="13.8">
+      <c r="A176" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B176" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C176" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="13.8">
+      <c r="A177" s="25" t="s">
+        <v>674</v>
+      </c>
+      <c r="B177" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C177" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="13.8">
+      <c r="A178" s="13" t="s">
+        <v>678</v>
+      </c>
+      <c r="B178" s="25" t="s">
+        <v>679</v>
+      </c>
+      <c r="C178" s="25" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" ht="13.8">
+      <c r="A179" s="25" t="s">
+        <v>683</v>
+      </c>
+      <c r="B179" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C179" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="13.8">
+      <c r="A180" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B180" s="13" t="s">
+        <v>685</v>
+      </c>
+      <c r="C180" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="13.8">
+      <c r="A181" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B181" s="25" t="s">
+        <v>687</v>
+      </c>
+      <c r="C181" s="25" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" ht="13.8">
+      <c r="A182" s="13" t="s">
+        <v>691</v>
+      </c>
+      <c r="B182" s="13" t="s">
+        <v>692</v>
+      </c>
+      <c r="C182" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" ht="13.8">
+      <c r="A183" s="13" t="s">
+        <v>695</v>
+      </c>
+      <c r="B183" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C183" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="13.8">
+      <c r="A184" s="13" t="s">
+        <v>698</v>
+      </c>
+      <c r="B184" s="25" t="s">
+        <v>699</v>
+      </c>
+      <c r="C184" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" ht="13.8">
+      <c r="A185" s="13" t="s">
+        <v>701</v>
+      </c>
+      <c r="B185" s="13" t="s">
+        <v>702</v>
+      </c>
+      <c r="C185" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" ht="13.8">
+      <c r="A186" s="13" t="s">
+        <v>705</v>
+      </c>
+      <c r="B186" s="25" t="s">
+        <v>706</v>
+      </c>
+      <c r="C186" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="13.8">
+      <c r="A187" s="13" t="s">
+        <v>709</v>
+      </c>
+      <c r="B187" s="25" t="s">
+        <v>710</v>
+      </c>
+      <c r="C187" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="13.8">
+      <c r="A188" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B188" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C188" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="13.8">
+      <c r="A189" s="25" t="s">
+        <v>715</v>
+      </c>
+      <c r="B189" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C189" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="13.8">
+      <c r="A190" s="13" t="s">
+        <v>718</v>
+      </c>
+      <c r="B190" s="25" t="s">
+        <v>719</v>
+      </c>
+      <c r="C190" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="13.8">
+      <c r="A191" s="13" t="s">
+        <v>723</v>
+      </c>
+      <c r="B191" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C191" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="13.8">
+      <c r="A192" s="13" t="s">
+        <v>727</v>
+      </c>
+      <c r="B192" s="13" t="s">
+        <v>728</v>
+      </c>
+      <c r="C192" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" ht="13.8">
+      <c r="A193" s="13" t="s">
+        <v>731</v>
+      </c>
+      <c r="B193" s="25" t="s">
+        <v>732</v>
+      </c>
+      <c r="C193" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" ht="13.8">
+      <c r="A194" s="13" t="s">
+        <v>736</v>
+      </c>
+      <c r="B194" s="25" t="s">
+        <v>737</v>
+      </c>
+      <c r="C194" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" ht="13.8">
+      <c r="A195" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="B195" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C195" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" ht="13.8">
+      <c r="A196" s="13" t="s">
+        <v>743</v>
+      </c>
+      <c r="B196" s="25" t="s">
+        <v>744</v>
+      </c>
+      <c r="C196" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" ht="13.8">
+      <c r="A197" s="13" t="s">
+        <v>748</v>
+      </c>
+      <c r="B197" s="13" t="s">
+        <v>749</v>
+      </c>
+      <c r="C197" s="13" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="13.8">
+      <c r="A198" s="13" t="s">
+        <v>754</v>
+      </c>
+      <c r="B198" s="13" t="s">
+        <v>755</v>
+      </c>
+      <c r="C198" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" ht="13.8">
+      <c r="A199" s="13" t="s">
+        <v>759</v>
+      </c>
+      <c r="B199" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C199" s="13" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" ht="13.8">
+      <c r="A200" s="13" t="s">
+        <v>764</v>
+      </c>
+      <c r="B200" s="13" t="s">
+        <v>765</v>
+      </c>
+      <c r="C200" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" ht="13.8">
+      <c r="A201" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B201" s="13" t="s">
+        <v>769</v>
+      </c>
+      <c r="C201" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="13.8">
+      <c r="A202" s="13" t="s">
+        <v>772</v>
+      </c>
+      <c r="B202" s="13" t="s">
+        <v>773</v>
+      </c>
+      <c r="C202" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="13.8">
+      <c r="A203" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B203" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C203" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="13.8">
+      <c r="A204" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B204" s="25" t="s">
+        <v>779</v>
+      </c>
+      <c r="C204" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" ht="13.8">
+      <c r="A205" s="13" t="s">
+        <v>783</v>
+      </c>
+      <c r="B205" s="25" t="s">
+        <v>784</v>
+      </c>
+      <c r="C205" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" ht="13.8">
+      <c r="A206" s="13" t="s">
+        <v>788</v>
+      </c>
+      <c r="B206" s="25" t="s">
+        <v>789</v>
+      </c>
+      <c r="C206" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" ht="13.8">
+      <c r="A207" s="25" t="s">
+        <v>793</v>
+      </c>
+      <c r="B207" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C207" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" ht="13.8">
+      <c r="A208" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B208" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C208" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="13.8">
+      <c r="A209" s="13" t="s">
+        <v>799</v>
+      </c>
+      <c r="B209" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C209" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" ht="13.8">
+      <c r="A210" s="13" t="s">
+        <v>803</v>
+      </c>
+      <c r="B210" s="13" t="s">
+        <v>804</v>
+      </c>
+      <c r="C210" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" ht="13.8">
+      <c r="A211" s="25" t="s">
+        <v>808</v>
+      </c>
+      <c r="B211" s="25" t="s">
+        <v>809</v>
+      </c>
+      <c r="C211" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" ht="13.8">
+      <c r="A212" s="25" t="s">
+        <v>813</v>
+      </c>
+      <c r="B212" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C212" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" ht="13.8">
+      <c r="A213" s="25" t="s">
+        <v>817</v>
+      </c>
+      <c r="B213" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C213" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" ht="13.8">
+      <c r="A214" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B214" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C214" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" ht="13.8">
+      <c r="A215" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B215" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C215" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" ht="13.8">
+      <c r="A216" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B216" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C216" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" ht="13.8">
+      <c r="A217" s="13" t="s">
+        <v>827</v>
+      </c>
+      <c r="B217" s="25" t="s">
+        <v>828</v>
+      </c>
+      <c r="C217" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" ht="13.8">
+      <c r="A218" s="13" t="s">
+        <v>826</v>
+      </c>
+      <c r="B218" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C218" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" ht="13.8">
+      <c r="A219" s="13" t="s">
+        <v>833</v>
+      </c>
+      <c r="B219" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C219" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" ht="13.8">
+      <c r="A220" s="13" t="s">
+        <v>837</v>
+      </c>
+      <c r="B220" s="25" t="s">
+        <v>838</v>
+      </c>
+      <c r="C220" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" ht="13.8">
+      <c r="A221" s="13" t="s">
+        <v>841</v>
+      </c>
+      <c r="B221" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C221" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" ht="13.8">
+      <c r="A222" s="13" t="s">
+        <v>845</v>
+      </c>
+      <c r="B222" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C222" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" ht="13.8">
+      <c r="A223" s="13" t="s">
+        <v>848</v>
+      </c>
+      <c r="B223" s="13" t="s">
+        <v>849</v>
+      </c>
+      <c r="C223" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" ht="13.8">
+      <c r="A224" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B224" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C224" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" ht="13.8">
+      <c r="A225" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B225" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C225" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" ht="13.8">
+      <c r="A226" s="13" t="s">
+        <v>857</v>
+      </c>
+      <c r="B226" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C226" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" ht="13.8">
+      <c r="A227" s="13" t="s">
+        <v>861</v>
+      </c>
+      <c r="B227" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C227" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" ht="13.8">
+      <c r="A228" s="13" t="s">
+        <v>865</v>
+      </c>
+      <c r="B228" s="13" t="s">
+        <v>866</v>
+      </c>
+      <c r="C228" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" ht="13.8">
+      <c r="A229" s="13" t="s">
+        <v>870</v>
+      </c>
+      <c r="B229" s="13" t="s">
+        <v>871</v>
+      </c>
+      <c r="C229" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" ht="13.8">
+      <c r="A230" s="13" t="s">
+        <v>875</v>
+      </c>
+      <c r="B230" s="13" t="s">
+        <v>876</v>
+      </c>
+      <c r="C230" s="27" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" ht="13.8">
+      <c r="A231" s="13" t="s">
+        <v>881</v>
+      </c>
+      <c r="B231" s="13" t="s">
+        <v>882</v>
+      </c>
+      <c r="C231" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" ht="13.8">
+      <c r="A232" s="13" t="s">
+        <v>885</v>
+      </c>
+      <c r="B232" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C232" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" ht="13.8">
+      <c r="A233" s="13" t="s">
+        <v>888</v>
+      </c>
+      <c r="B233" s="13" t="s">
+        <v>889</v>
+      </c>
+      <c r="C233" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" ht="13.8">
+      <c r="A234" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B234" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C234" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" ht="13.8">
+      <c r="A235" s="13" t="s">
+        <v>895</v>
+      </c>
+      <c r="B235" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C235" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" ht="13.8">
+      <c r="A236" s="25" t="s">
+        <v>899</v>
+      </c>
+      <c r="B236" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C236" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" ht="13.8">
+      <c r="A237" s="13" t="s">
+        <v>903</v>
+      </c>
+      <c r="B237" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C237" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" ht="13.8">
+      <c r="A238" s="13" t="s">
+        <v>907</v>
+      </c>
+      <c r="B238" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C238" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" ht="13.8">
+      <c r="A239" s="13" t="s">
+        <v>910</v>
+      </c>
+      <c r="B239" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C239" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" ht="13.8">
+      <c r="A240" s="25" t="s">
+        <v>913</v>
+      </c>
+      <c r="B240" s="13" t="s">
+        <v>914</v>
+      </c>
+      <c r="C240" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" ht="13.8">
+      <c r="A241" s="13" t="s">
+        <v>916</v>
+      </c>
+      <c r="B241" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C241" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" ht="13.8">
+      <c r="A242" s="25" t="s">
+        <v>919</v>
+      </c>
+      <c r="B242" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C242" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" ht="13.8">
+      <c r="A243" s="13" t="s">
+        <v>922</v>
+      </c>
+      <c r="B243" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C243" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" ht="13.8">
+      <c r="A244" s="25" t="s">
+        <v>925</v>
+      </c>
+      <c r="B244" s="25" t="s">
+        <v>926</v>
+      </c>
+      <c r="C244" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" ht="13.8">
+      <c r="A245" s="13" t="s">
+        <v>929</v>
+      </c>
+      <c r="B245" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C245" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" ht="13.8">
+      <c r="A246" s="13" t="s">
+        <v>933</v>
+      </c>
+      <c r="B246" s="13" t="s">
+        <v>934</v>
+      </c>
+      <c r="C246" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" ht="13.8">
+      <c r="A247" s="25" t="s">
+        <v>938</v>
+      </c>
+      <c r="B247" s="13" t="s">
+        <v>939</v>
+      </c>
+      <c r="C247" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" ht="13.8">
+      <c r="A248" s="25" t="s">
+        <v>943</v>
+      </c>
+      <c r="B248" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C248" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" ht="13.8">
+      <c r="A249" s="36" t="s">
+        <v>946</v>
+      </c>
+      <c r="B249" s="13" t="s">
+        <v>947</v>
+      </c>
+      <c r="C249" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" ht="13.8">
+      <c r="A250" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B250" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C250" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" ht="13.8">
+      <c r="A251" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B251" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C251" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" ht="13.8">
+      <c r="A252" s="13" t="s">
+        <v>955</v>
+      </c>
+      <c r="B252" s="13" t="s">
+        <v>956</v>
+      </c>
+      <c r="C252" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" ht="13.8">
+      <c r="A253" s="13" t="s">
+        <v>960</v>
+      </c>
+      <c r="B253" s="25" t="s">
+        <v>961</v>
+      </c>
+      <c r="C253" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" ht="13.8">
+      <c r="A254" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B254" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C254" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" ht="13.8">
+      <c r="A255" s="13" t="s">
+        <v>967</v>
+      </c>
+      <c r="B255" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C255" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" ht="13.8">
+      <c r="A256" s="13" t="s">
+        <v>970</v>
+      </c>
+      <c r="B256" s="25" t="s">
+        <v>971</v>
+      </c>
+      <c r="C256" s="13" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" ht="13.8">
+      <c r="A257" s="36" t="s">
+        <v>976</v>
+      </c>
+      <c r="B257" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C257" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" ht="13.8">
+      <c r="A258" s="36" t="s">
+        <v>979</v>
+      </c>
+      <c r="B258" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C258" s="13" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" ht="13.8">
+      <c r="A259" s="36" t="s">
+        <v>983</v>
+      </c>
+      <c r="B259" s="13" t="s">
+        <v>984</v>
+      </c>
+      <c r="C259" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" ht="13.8">
+      <c r="A260" s="36" t="s">
+        <v>987</v>
+      </c>
+      <c r="B260" s="25" t="s">
+        <v>988</v>
+      </c>
+      <c r="C260" s="25" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" ht="13.8">
+      <c r="A261" s="36" t="s">
+        <v>991</v>
+      </c>
+      <c r="B261" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C261" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" ht="13.8">
+      <c r="A262" s="13" t="s">
+        <v>994</v>
+      </c>
+      <c r="B262" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C262" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" ht="13.8">
+      <c r="A263" s="13" t="s">
+        <v>997</v>
+      </c>
+      <c r="B263" s="25" t="s">
+        <v>998</v>
+      </c>
+      <c r="C263" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" ht="13.8">
+      <c r="A264" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B264" s="13" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C264" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" ht="13.8">
+      <c r="A265" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B265" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C265" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" ht="13.8">
+      <c r="A266" s="13" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B266" s="13" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C266" s="36" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" ht="13.8">
+      <c r="A267" s="13" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B267" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C267" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" ht="13.8">
+      <c r="A268" s="29" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B268" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C268" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" ht="13.8">
+      <c r="A269" s="13" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B269" s="13" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C269" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" ht="13.8">
+      <c r="A270" s="13" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B270" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C270" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" ht="13.8">
+      <c r="A271" s="13" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B271" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C271" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" ht="13.8">
+      <c r="A272" s="29" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B272" s="29" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C272" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" ht="13.8">
+      <c r="A273" s="36" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B273" s="13" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C273" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" ht="158.4">
+      <c r="A274" s="13" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B274" s="30" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C274" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" ht="13.8">
+      <c r="A275" s="36" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B275" s="31" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C275" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" ht="13.8">
+      <c r="A276" s="29" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B276" s="13" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C276" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" ht="13.8">
+      <c r="A277" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B277" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C277" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" ht="13.8">
+      <c r="A278" s="29" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B278" s="29" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C278" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" ht="13.8">
+      <c r="A279" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B279" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C279" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" ht="13.8">
+      <c r="A280" s="13" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B280" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C280" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" ht="13.8">
+      <c r="A281" s="29" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B281" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C281" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" ht="13.8">
+      <c r="A282" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B282" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C282" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" ht="13.8">
+      <c r="A283" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B283" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C283" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" ht="13.8">
+      <c r="A284" s="13" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B284" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C284" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" ht="13.8">
+      <c r="A285" s="13" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B285" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C285" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" ht="13.8">
+      <c r="A286" s="13" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B286" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C286" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" ht="13.8">
+      <c r="A287" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B287" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C287" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" ht="13.8">
+      <c r="A288" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B288" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C288" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" ht="13.8">
+      <c r="A289" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B289" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C289" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{EE160D9A-37A2-4933-8E76-88E346485FB0}"/>
+    <hyperlink ref="B1" r:id="rId2" xr:uid="{E0A1DEA4-4D08-46D1-9461-92E872D93AC6}"/>
+    <hyperlink ref="C1" r:id="rId3" xr:uid="{905DBC65-6147-4C6D-A219-FBFDF8E1F919}"/>
+    <hyperlink ref="A2" r:id="rId4" xr:uid="{956BE504-D62D-484F-B13C-DDC2BD2792F4}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{4FA962B9-AA6D-40ED-9F9E-3A734CA5303F}"/>
+    <hyperlink ref="A4" r:id="rId6" xr:uid="{A3037E59-A60F-4263-8734-9D6B3639A415}"/>
+    <hyperlink ref="B4" r:id="rId7" xr:uid="{FEC9BE41-1CB0-456A-B884-552A2392F597}"/>
+    <hyperlink ref="A8" r:id="rId8" xr:uid="{C6BFB3DB-6303-4C5B-A414-B4B0477BC4EB}"/>
+    <hyperlink ref="B8" r:id="rId9" xr:uid="{787334D0-34C1-48D7-8B5A-1D4A5AF5992C}"/>
+    <hyperlink ref="C8" r:id="rId10" xr:uid="{4E345C5A-3CF8-43BD-B119-B883430C2F4C}"/>
+    <hyperlink ref="A9" r:id="rId11" xr:uid="{C19F4236-5D83-4663-8192-8E33D4879ECF}"/>
+    <hyperlink ref="C9" r:id="rId12" xr:uid="{50D69FBC-15D6-4C56-8673-F95B4FA94291}"/>
+    <hyperlink ref="C10" r:id="rId13" xr:uid="{2C4AF700-D562-4576-BAD5-D60B01850A8A}"/>
+    <hyperlink ref="A11" r:id="rId14" xr:uid="{4A0182A2-94CC-4213-A557-30EF3F642850}"/>
+    <hyperlink ref="A15" r:id="rId15" xr:uid="{1C9B1101-39AA-437A-9997-0478B9DE4228}"/>
+    <hyperlink ref="A16" r:id="rId16" xr:uid="{A9495E6A-8E07-4EA0-98C8-1DFEAC997359}"/>
+    <hyperlink ref="B16" r:id="rId17" display="https://www.healthgrades.com/physician/dr-amy-chen-x4768" xr:uid="{72DB2C01-8B7A-41D0-A9F2-09D083E53446}"/>
+    <hyperlink ref="C16" r:id="rId18" xr:uid="{F5B1EB45-677E-4011-B7CD-EC7B338D751B}"/>
+    <hyperlink ref="A19" r:id="rId19" xr:uid="{CC0D361A-6998-4329-8AA0-C7DDDECB134A}"/>
+    <hyperlink ref="A20" r:id="rId20" xr:uid="{D9EDFA1E-203F-4057-B529-DD893C5E236E}"/>
+    <hyperlink ref="B20" r:id="rId21" xr:uid="{4B0D689E-8610-48E2-9EF3-745D2C6E7955}"/>
+    <hyperlink ref="A22" r:id="rId22" xr:uid="{1FE00AD4-7B91-41F9-85C8-60369DCC3305}"/>
+    <hyperlink ref="B22" r:id="rId23" xr:uid="{E1E269FB-F83A-4895-8F19-85F0E24A3C76}"/>
+    <hyperlink ref="A23" r:id="rId24" xr:uid="{10B20308-3792-4BF1-B7AC-EB4317225136}"/>
+    <hyperlink ref="A24" r:id="rId25" xr:uid="{3E8FB6E2-0FB9-4CF6-A5F4-2A505561089D}"/>
+    <hyperlink ref="B24" r:id="rId26" xr:uid="{6467A46B-9DAD-409C-ABE2-ABC78BA3A5CA}"/>
+    <hyperlink ref="A25" r:id="rId27" xr:uid="{4B8C008B-1780-4B42-8E63-879D95917D4E}"/>
+    <hyperlink ref="B25" r:id="rId28" xr:uid="{F0370970-0079-44A4-803B-E032C10ED2F6}"/>
+    <hyperlink ref="A26" r:id="rId29" xr:uid="{369871F2-ED5C-4B92-A3E2-98410063C6F5}"/>
+    <hyperlink ref="A27" r:id="rId30" xr:uid="{FE81B9CA-9F3C-4371-BAD2-E1115801F957}"/>
+    <hyperlink ref="B27" r:id="rId31" xr:uid="{68E5B309-EEEC-43CF-B890-B519681E95FE}"/>
+    <hyperlink ref="C27" r:id="rId32" xr:uid="{2C2DBA41-56D9-45C5-B345-515D0C48184D}"/>
+    <hyperlink ref="A28" r:id="rId33" xr:uid="{EDA58CBC-B779-4220-8B11-4D4FB3F48ED6}"/>
+    <hyperlink ref="B28" r:id="rId34" xr:uid="{AEFDEA78-CBFA-4448-B539-61C1E8FF4979}"/>
+    <hyperlink ref="B31" r:id="rId35" xr:uid="{7F44EA46-008B-4E4B-A881-877AB3F42449}"/>
+    <hyperlink ref="A33" r:id="rId36" xr:uid="{A9136A79-7EAD-442C-8A8E-B1799F4BDDA3}"/>
+    <hyperlink ref="B33" r:id="rId37" xr:uid="{57FABAC3-4D92-4B7B-BA2E-D11C873B1FE7}"/>
+    <hyperlink ref="A34" r:id="rId38" xr:uid="{92A66E94-ABAB-4272-AF9F-DD400284A1C1}"/>
+    <hyperlink ref="A39" r:id="rId39" xr:uid="{CCB674E9-F96B-489E-BCB0-135E76A500A9}"/>
+    <hyperlink ref="B39" r:id="rId40" xr:uid="{D0817D6E-3AC4-49BB-872B-180853FE9F91}"/>
+    <hyperlink ref="C39" r:id="rId41" xr:uid="{C8B08FF8-9B1F-4CDB-804D-DA8AD6E507DC}"/>
+    <hyperlink ref="A41" r:id="rId42" xr:uid="{51194BD8-6076-4754-BD0C-DD45E6148DEE}"/>
+    <hyperlink ref="B41" r:id="rId43" xr:uid="{58081544-3BB1-4245-A5B0-A0E040DBD418}"/>
+    <hyperlink ref="C41" r:id="rId44" xr:uid="{18746CC5-4640-47E7-ABB6-0E9D40F60761}"/>
+    <hyperlink ref="A42" r:id="rId45" xr:uid="{CCD0AEF2-AD1B-49B2-BC18-E80CF4E5EC95}"/>
+    <hyperlink ref="A100" r:id="rId46" xr:uid="{3FA91BD9-D4C7-43E5-A22F-DF335B29824B}"/>
+    <hyperlink ref="B274" r:id="rId47" xr:uid="{FB7CA805-4020-4ACD-8D56-AB29BD4F8D7F}"/>
+    <hyperlink ref="A61" r:id="rId48" xr:uid="{519C357B-E92D-40F3-9407-473DE1431313}"/>
+    <hyperlink ref="C87" r:id="rId49" xr:uid="{A6A0FF55-6D25-4B99-B4D0-906231B7E00D}"/>
+    <hyperlink ref="C266" r:id="rId50" xr:uid="{38DA9241-7268-412E-9529-F210A255DBE9}"/>
+    <hyperlink ref="A275" r:id="rId51" xr:uid="{279CE7ED-EAB3-4AD4-B7EE-4CFBBACBA23D}"/>
+    <hyperlink ref="A273" r:id="rId52" xr:uid="{2817575E-41D9-4E6C-B20E-B182D1617F44}"/>
+    <hyperlink ref="A249" r:id="rId53" xr:uid="{2D38FF34-C4DB-4D0E-AF22-E3CB69ABF2A2}"/>
+    <hyperlink ref="A261" r:id="rId54" xr:uid="{8C3910B1-3C09-46FC-A7E4-405710B63879}"/>
+    <hyperlink ref="A260" r:id="rId55" xr:uid="{51FED39B-346C-458F-9474-322AA9FC4A3F}"/>
+    <hyperlink ref="A259" r:id="rId56" xr:uid="{2D073FBE-0196-4723-ACAE-FB7F930DD8CB}"/>
+    <hyperlink ref="A257" r:id="rId57" xr:uid="{F6FD9E34-5585-4CE4-8E08-7B14EC2F2510}"/>
+    <hyperlink ref="A258" r:id="rId58" xr:uid="{D7240623-B27A-4A92-B924-CDE2CCE0716F}"/>
+    <hyperlink ref="B47" r:id="rId59" xr:uid="{1EB5CC58-FE3D-4122-AED8-1CD01CA354F2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId60"/>
+</worksheet>
 </file>
</xml_diff>